<commit_message>
Fixed image handling for questions
</commit_message>
<xml_diff>
--- a/questions3.xlsx
+++ b/questions3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F82F323-990B-4070-A5FF-0BBA9FDFF59B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE5B02A-2E68-4A5B-886A-3A1B65503438}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="237">
   <si>
     <t>Question</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Вибухові речовини це…</t>
-  </si>
-  <si>
-    <t>хімічні з’єднання або суміші, які під впливом визначених зовнішніх впливів здатні до швидкого само розповсюдженого хімічного перетворення із утворенням сильно нагрітих газів, що володіють великим тиском, які, розширюючись, виконують механічну роботу</t>
   </si>
   <si>
     <t>речовини, які вибухають від тертя або нагрівання</t>
@@ -286,13 +283,498 @@
     </r>
   </si>
   <si>
-    <t>підриву поодиноких зарядів ВР або для різного за часом підриву серій зарядів, коли вибух одного з них не може пошкодити інший заряд або іншої серії</t>
-  </si>
-  <si>
     <t>здійснення одночасного вибуху декількох зарядів, а також для бескапсюльного підриву зарядів вибухових речовин</t>
   </si>
   <si>
-    <t>одночасного вибуху декількох зарядів або для виконання вибуху в точно встановлений час</t>
+    <t>хімічні речовини, здатні під впливом зовнішніх дій до швидкого хімічного перетворення, що відбувається з виділенням великої кількості тепла і газоподібних продуктів</t>
+  </si>
+  <si>
+    <t>До яких зарядів відноситься це визначення? 
+"Заряди, форма яких наближається до куба чи паралелепіпеда, довжина якого не перевищує його найменший поперечний вимір більше ніж у п’ять разів"</t>
+  </si>
+  <si>
+    <t>зосереджені заряди</t>
+  </si>
+  <si>
+    <t>кумулятивні заряди</t>
+  </si>
+  <si>
+    <t>подовжені заряди</t>
+  </si>
+  <si>
+    <t>фігурні заряди</t>
+  </si>
+  <si>
+    <t>До яких зарядів відноситься це визначення? 
+"Заряди, що мають різноманітну форму і
+використовуються для підривання різних фігурних елементів конструкцій"</t>
+  </si>
+  <si>
+    <t>До яких зарядів відноситься це визначення? 
+"Заряди, які мають форму витягнутих паралелепіпедів
+чи циліндрів, довжина яких більше ніж у п’ять разів перевищує їх найменші
+поперечні розміри, при цьому висота зарядів, що мають форму
+паралелепіпедів, не повинна перевищувати їх ширину"</t>
+  </si>
+  <si>
+    <t>За формою заряди бувають</t>
+  </si>
+  <si>
+    <t>великокаліберні заряди</t>
+  </si>
+  <si>
+    <t>індукційні заряди</t>
+  </si>
+  <si>
+    <t>підривання поодиноких зарядів ВР і для різночасового підривання серій зарядів, коли підривання одного з них не може пошкодити інший заряд чи іншу серію</t>
+  </si>
+  <si>
+    <t>Які засоби підривання використовуються при вогневому способі</t>
+  </si>
+  <si>
+    <t>вогнепровідний шнур</t>
+  </si>
+  <si>
+    <t>детонуючий шнур</t>
+  </si>
+  <si>
+    <t>капсулі-детонатори</t>
+  </si>
+  <si>
+    <t>запалювальні трубки</t>
+  </si>
+  <si>
+    <t>електродетонатори</t>
+  </si>
+  <si>
+    <t>Яка довжина бухти вогнепровідного шнура</t>
+  </si>
+  <si>
+    <t>5 метрів</t>
+  </si>
+  <si>
+    <t>20 метрів</t>
+  </si>
+  <si>
+    <t>15 метрів</t>
+  </si>
+  <si>
+    <t>25 метрів</t>
+  </si>
+  <si>
+    <t>50 метрів</t>
+  </si>
+  <si>
+    <t>10 метрів</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Вогнепровідний шнур складається з</t>
+  </si>
+  <si>
+    <t>порохової серцевини з
+однією направляючою ниткою всередині внутрішніх і зовнішніх обплетень і
+оболонки</t>
+  </si>
+  <si>
+    <t>Швидкість горіння вогнепровідного шнура на відкритому повітрі становить приблизно</t>
+  </si>
+  <si>
+    <t>1 см/с</t>
+  </si>
+  <si>
+    <t>10 см/с</t>
+  </si>
+  <si>
+    <t>1 м/с</t>
+  </si>
+  <si>
+    <t>10 м/с</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Горіння вогнепровідного шнура під водою протікає </t>
+  </si>
+  <si>
+    <t>швидше</t>
+  </si>
+  <si>
+    <t>повільніше</t>
+  </si>
+  <si>
+    <t>Перед використанням ВШ оглядають, і якщо на поверхні його оболонки є тріщини, переломи, сліди відмокання, розкувйовдження та інші пошкодження й несправності, то такий шнур вважається непридатним для роботи; кінці шнура в бухті довжиною по ___–___ см відрізають та спалюють. Швидкість горіння ВШ перевіряють підпалюванням його відрізка довжиною ___ см, визначаючи час горіння за секундоміром чи за годинником із секундною стрілкою. Час горіння відрізка вказаної довжини повинен становити ___–___ секунд.</t>
+  </si>
+  <si>
+    <t>fillblank</t>
+  </si>
+  <si>
+    <t>Виготовлення ЗТП відбувається в такому порядку:</t>
+  </si>
+  <si>
+    <t>чистим гострим ножем на дерев’яній підкладці відрізають під прямим кутом шматок ВШ необхідної довжини</t>
+  </si>
+  <si>
+    <t>виймають із коробки КД і перевіряють його придатність шляхом огляду</t>
+  </si>
+  <si>
+    <t>закріплюють КД на ВШ спеціальним обтискачем, для чого беруть шнур у
+ліву руку і, притримуючи КД вказівним пальцем, накладають правою рукою обтискач так, щоб його нижня поверхня була на рівні зрізу гільзи; поступово посилюючи натискання на обтискач і повертаючи його, створюють біля краю гільзи кільцеву шийку, таким чином досягається міцність з’єднання КД зі шнуром</t>
+  </si>
+  <si>
+    <t>обрізаний під прямим кутом кінець ВШ обережно вводять у гільзу КД до
+упору в чашечку. Шнур повинен входити в гільзу легко, без натискання і обертання, які можуть призвести до підривання КД. Якщо шнур входить у гільзу досить вільно, його кінець обгортають одним шаром ізоляційної стрічки чи паперу</t>
+  </si>
+  <si>
+    <t>ordering</t>
+  </si>
+  <si>
+    <t>Характеристики ЗТП-50</t>
+  </si>
+  <si>
+    <t>matching</t>
+  </si>
+  <si>
+    <t>Час сповільнення вибуху у повітрі, с</t>
+  </si>
+  <si>
+    <t>Час сповільнення вибуху у воді на глибині 5 м, с</t>
+  </si>
+  <si>
+    <t>Довжина, см</t>
+  </si>
+  <si>
+    <t>Маса, г</t>
+  </si>
+  <si>
+    <t>Колір ВШ</t>
+  </si>
+  <si>
+    <t>сірувато-білий</t>
+  </si>
+  <si>
+    <t>Характеристики ЗТП-150</t>
+  </si>
+  <si>
+    <t>Характеристики ЗТП-300</t>
+  </si>
+  <si>
+    <t>блакитний</t>
+  </si>
+  <si>
+    <t>Під час використання ЗТП з механічним запалювачем необхідно:</t>
+  </si>
+  <si>
+    <t>переконатися, що чека знаходиться в глибокому прорізі</t>
+  </si>
+  <si>
+    <t>накрутити запалювач на ніпель запалювального вузла ЗТП</t>
+  </si>
+  <si>
+    <t>вкрутити КД у запалювальне гніздо заряду</t>
+  </si>
+  <si>
+    <t>трохи підняти і поворотом на 90º переставити чеку з глибокого прорізу в
+мілкий</t>
+  </si>
+  <si>
+    <t>тримаючи запалювач лівою рукою за корпус, правою рукою висмикнути
+чеку за кільце (шток запалювача направити при цьому від себе)</t>
+  </si>
+  <si>
+    <t>Детонуючий шнур складається з</t>
+  </si>
+  <si>
+    <t>серцевини бризантної ВР (тену) з двома направляючими нитками і ряду внутрішніх і зовнішніх обплетень, покритих вологоізолюючою оболонкою</t>
+  </si>
+  <si>
+    <t>Діаметр ДШ дорівнює ___–___ мм. ДШ підривається зі швидкістю не менше ___ метрів за секунду. Його
+слід оберігати від механічних пошкоджень, а також від дії вологи і вогню; від вогню ДШ може загоратися і повільно горіти; у разі прострілювання кулею він
+може детонувати. ДШ відрізками довжиною ___ м зберігається згорнутим у бухти з покритими мастикою кінцями в сухих прохолодних приміщеннях окремо від ВШ і зарядів. Під водою ДШ марки ДШ-В можна підривати за умови перебування його
+там не більше ___ годин</t>
+  </si>
+  <si>
+    <t>4-5 витків</t>
+  </si>
+  <si>
+    <t>Скількома витками детонуючого шнура необхідно обмотати шашку пресованого
+тротилу щоб можна було підірвати її без КД?</t>
+  </si>
+  <si>
+    <t>2-3 витка</t>
+  </si>
+  <si>
+    <t>3-4 витка</t>
+  </si>
+  <si>
+    <t>Picture 31</t>
+  </si>
+  <si>
+    <t>послідовний</t>
+  </si>
+  <si>
+    <t>вистачить одного витка</t>
+  </si>
+  <si>
+    <t>послідовна</t>
+  </si>
+  <si>
+    <t>паралельна</t>
+  </si>
+  <si>
+    <t>пучкова</t>
+  </si>
+  <si>
+    <t>змішана</t>
+  </si>
+  <si>
+    <t>Picture 32</t>
+  </si>
+  <si>
+    <t>Picture 33</t>
+  </si>
+  <si>
+    <t>одночасного підривання кількох зарядів чи для проведення підривання в точно встановлений час</t>
+  </si>
+  <si>
+    <t>Електричний спосіб підривання використовується для</t>
+  </si>
+  <si>
+    <t>проводи</t>
+  </si>
+  <si>
+    <t>джерела струму</t>
+  </si>
+  <si>
+    <t>перевірочні та вимірювальні прилади</t>
+  </si>
+  <si>
+    <t>Які засоби підривання використовуються при електричному способі</t>
+  </si>
+  <si>
+    <t>Характеристики ЕДП (ЭДП-р)</t>
+  </si>
+  <si>
+    <t>опір у холодному стані</t>
+  </si>
+  <si>
+    <t>від 0,9 до 1,5 Ом</t>
+  </si>
+  <si>
+    <t>розрахунковий опір у нагрітому стані (під час підривання) разом з
+відвідними проводами довжиною 1 м</t>
+  </si>
+  <si>
+    <t>2,5 Ом</t>
+  </si>
+  <si>
+    <t>мінімальний запалювальний струм</t>
+  </si>
+  <si>
+    <t>0,4 А</t>
+  </si>
+  <si>
+    <t>мінімальний розрахунковий струм для підривання одиничного ЕДП при постійному струмі</t>
+  </si>
+  <si>
+    <t>0,5 А</t>
+  </si>
+  <si>
+    <t>мінімальний розрахунковий струм для підривання одиничного ЕДП при змінному струмі</t>
+  </si>
+  <si>
+    <t>1 А</t>
+  </si>
+  <si>
+    <t>безпечний струм</t>
+  </si>
+  <si>
+    <t>0,18 А</t>
+  </si>
+  <si>
+    <t>Яка схема електро-вибухової мережі зображена на малюнку?</t>
+  </si>
+  <si>
+    <t>Який вид мережі ДШ зображена на малюнку?</t>
+  </si>
+  <si>
+    <t>з послідовним з’єднанням ЕДП</t>
+  </si>
+  <si>
+    <t>з послідовним з’єднанням груп, що складаються з попарнопаралельно з’єднаних ЕДП</t>
+  </si>
+  <si>
+    <t>з паралельно-пучковим з’єднанням ЕДП</t>
+  </si>
+  <si>
+    <t>зі змішаним з’єднанням ЕДП</t>
+  </si>
+  <si>
+    <t>Picture 34</t>
+  </si>
+  <si>
+    <t>Picture 35</t>
+  </si>
+  <si>
+    <t>Picture 36</t>
+  </si>
+  <si>
+    <t>U = I * R</t>
+  </si>
+  <si>
+    <t>I = U * R</t>
+  </si>
+  <si>
+    <t>R = U * I</t>
+  </si>
+  <si>
+    <t>I = R / U</t>
+  </si>
+  <si>
+    <t>Picture 37</t>
+  </si>
+  <si>
+    <t>Який вираз має закон Ома?</t>
+  </si>
+  <si>
+    <t>щоб запобігти розриванню зрощень</t>
+  </si>
+  <si>
+    <t>Запобіжна петля на ділянці зрощення саперного проводу використовується для</t>
+  </si>
+  <si>
+    <t>збільшення опору мережі</t>
+  </si>
+  <si>
+    <t>запобіганню розривання зрощень</t>
+  </si>
+  <si>
+    <t>зменшення опору мережі</t>
+  </si>
+  <si>
+    <t>маркування кінців мережі</t>
+  </si>
+  <si>
+    <t>Яка безпечна відстань для відкритого розміщення людей під час підривання зарядів до 10 кг без оболонок на ґрунті?</t>
+  </si>
+  <si>
+    <t>100 метрів</t>
+  </si>
+  <si>
+    <t>350 метрів</t>
+  </si>
+  <si>
+    <t>500 метрів</t>
+  </si>
+  <si>
+    <t>Яка безпечна відстань для відкритого розміщення людей під час підривання під час підривання відкрито розміщених металевих конструкцій зарядами до 10 кг без оболонок?</t>
+  </si>
+  <si>
+    <t>Яка безпечна відстань для відкритого розміщення людей під час підривання  цегли, каменю, бетону і залізобетону зарядами до 10 кг без оболонок?</t>
+  </si>
+  <si>
+    <t>Не ближче якої відстані дозволяється палити, розводити вогонь і запалювати багаття від місця виконання робіт з вибуховими речовинами та засобами підриву?</t>
+  </si>
+  <si>
+    <t>15 хвилин</t>
+  </si>
+  <si>
+    <t>5 хвилин</t>
+  </si>
+  <si>
+    <t>10 хвилин</t>
+  </si>
+  <si>
+    <t>30 хвилин</t>
+  </si>
+  <si>
+    <t>Не раніше ніж через який час із того моменту, коли за підрахунками повинен був відбутися вибух, можна підходити до зарядів, що відмовили при вогневому способі підривання?</t>
+  </si>
+  <si>
+    <t>порохової серцевини всередені та направляючого стрижня з бризантної ВР навколо неї</t>
+  </si>
+  <si>
+    <t>серцевини бризантної ВР та пороху покритих вологоізолюючою оболонкою</t>
+  </si>
+  <si>
+    <t>Основні тактико-технічні характеристики протипіхотної міни МОН-50</t>
+  </si>
+  <si>
+    <t>Маса</t>
+  </si>
+  <si>
+    <t>2 кг</t>
+  </si>
+  <si>
+    <t>Маса заряду</t>
+  </si>
+  <si>
+    <t>0,7 кг</t>
+  </si>
+  <si>
+    <t>Тип заряду</t>
+  </si>
+  <si>
+    <t>ПВВ-5А</t>
+  </si>
+  <si>
+    <t>Горизонтальний кут розкидання осколків</t>
+  </si>
+  <si>
+    <t>54°</t>
+  </si>
+  <si>
+    <t>Радіус суцільного ураження</t>
+  </si>
+  <si>
+    <t>50 / 58 м</t>
+  </si>
+  <si>
+    <t>Ширина зони суцільного ураження на відстані 50 / 58 м</t>
+  </si>
+  <si>
+    <t>45 / 54 м</t>
+  </si>
+  <si>
+    <t>Дальність ураження легкового та вантажного автотранспорту та живої сили в ньому</t>
+  </si>
+  <si>
+    <t>до 30 м</t>
+  </si>
+  <si>
+    <t>Дальність розльоту осколків від корпусу у тиловому та бічному напрямах</t>
+  </si>
+  <si>
+    <t>до 40 м</t>
+  </si>
+  <si>
+    <t>Дальність польоту забійних осколків</t>
+  </si>
+  <si>
+    <t>80 / 85 м</t>
+  </si>
+  <si>
+    <t>Порядок встановлення міни МОН-50 в грунт</t>
+  </si>
+  <si>
+    <t>послабити пробку одного запального гнізда</t>
+  </si>
+  <si>
+    <t>повернути міну опуклою стороною (стрілкою на прицілі) в напрямку цілі</t>
+  </si>
+  <si>
+    <t>відкинути ніжки вниз, розвести їх в сторони і втиснути в грунт на глибину, що забезпечує міні
+стійке положення</t>
+  </si>
+  <si>
+    <t>користуючись прицільною щілиною, навести міну на ціль (віху або місцевий предмет, який перебуває на місці очікуваної цілі), при наведенні відстань від ока навідника до щілини повинно бути 140-150 мм, лінія прицілювання повинна йти від ока навідника через середину жолоба на рівні нижньої площини щілини на центр цілі, для надання міні необхідного положення вона повертається на шарнірах і ніжках вдавлюється в ґрунт на необхідну глибину</t>
+  </si>
+  <si>
+    <t>вкрутити в запальний гніздо електродетонатор, приєднаний до дротової мережі управління, перевірити правильність прицілювання</t>
+  </si>
+  <si>
+    <t>замаскувати міну місцевим матеріалом (травою, гілками)</t>
+  </si>
+  <si>
+    <t>Для прицілювання міни МОН-50, якщо дозволяє час, використовується віха, що виготовляється у військах,
+яка встановлюється на напрямку руху, центру очікуваної групової цілі. Висота віхи від поверхні землі до поперечної планки при відстані ___ м – ___ м, при відстані ___ м – ___ м</t>
   </si>
 </sst>
 </file>
@@ -349,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -363,6 +845,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,16 +1067,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC22"/>
+  <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="2"/>
-    <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="30" style="2" customWidth="1"/>
     <col min="5" max="5" width="35" style="2" customWidth="1"/>
@@ -690,27 +1175,27 @@
         <v>8</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="225" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="131.25" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -724,7 +1209,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB2" s="2">
         <v>2</v>
@@ -732,52 +1217,52 @@
     </row>
     <row r="3" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="K3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
@@ -795,57 +1280,57 @@
         <v>2</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="K4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -863,57 +1348,57 @@
         <v>2</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="K5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="O5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -931,27 +1416,27 @@
         <v>2</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="75" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -965,7 +1450,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB6" s="2">
         <v>2</v>
@@ -973,37 +1458,37 @@
     </row>
     <row r="7" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1020,32 +1505,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3" t="s">
-        <v>66</v>
+        <v>85</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1059,54 +1536,37 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="AC8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>86</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="O9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>75</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -1115,29 +1575,34 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="4" t="s">
-        <v>9</v>
+      <c r="AA9" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="AB9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" ht="150" x14ac:dyDescent="0.3">
+      <c r="AC9" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="131.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="O10" s="3" t="s">
-        <v>80</v>
+      <c r="F10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1151,22 +1616,49 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="AC10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -1175,15 +1667,40 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
-      <c r="AA11" s="4"/>
-    </row>
-    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="AA11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
@@ -1195,18 +1712,55 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="4"/>
+      <c r="AA12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1215,15 +1769,30 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="4"/>
-    </row>
-    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="AA13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="168.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
@@ -1235,14 +1804,53 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="4"/>
-    </row>
-    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="AA14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -1251,11 +1859,32 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="4"/>
-    </row>
-    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="AA15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -1267,11 +1896,38 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="4"/>
-    </row>
-    <row r="17" spans="2:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="AA16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
@@ -1283,15 +1939,32 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="4"/>
-    </row>
-    <row r="18" spans="2:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="AA17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -1303,11 +1976,28 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="4"/>
-    </row>
-    <row r="19" spans="2:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="AA18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
@@ -1319,15 +2009,32 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="4"/>
-    </row>
-    <row r="20" spans="2:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="AA19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="206.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="O20" s="3">
+        <v>10</v>
+      </c>
+      <c r="P20" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>60</v>
+      </c>
+      <c r="R20" s="3">
+        <v>60</v>
+      </c>
+      <c r="S20" s="3">
+        <v>70</v>
+      </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -1335,35 +2042,994 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="4"/>
-    </row>
-    <row r="21" spans="2:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="AA20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="318.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
-    </row>
-    <row r="22" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O22" s="3">
+        <v>50</v>
+      </c>
+      <c r="P22" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q22">
+        <v>55</v>
+      </c>
+      <c r="R22">
+        <v>50</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O23" s="3">
+        <v>150</v>
+      </c>
+      <c r="P23" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q23">
+        <v>150</v>
+      </c>
+      <c r="R23">
+        <v>75</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB23" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O24" s="3">
+        <v>360</v>
+      </c>
+      <c r="P24" s="3">
+        <v>300</v>
+      </c>
+      <c r="Q24">
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <v>65</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="150" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="O26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="AA26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="O27" s="2">
+        <v>5</v>
+      </c>
+      <c r="P27" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>6500</v>
+      </c>
+      <c r="R27" s="2">
+        <v>50</v>
+      </c>
+      <c r="S27" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC30" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="173.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="155.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA35" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC35" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC36" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB41" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC41" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA45" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB45" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA46" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB46" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O47" s="2">
+        <v>10</v>
+      </c>
+      <c r="P47" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>30</v>
+      </c>
+      <c r="R47" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="AA47" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB47" s="5">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added percentage and duration formatting to admin results page
</commit_message>
<xml_diff>
--- a/questions3.xlsx
+++ b/questions3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE5B02A-2E68-4A5B-886A-3A1B65503438}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772B471-D0BA-4DD4-A429-E760172FA9A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="236">
   <si>
     <t>Question</t>
   </si>
@@ -634,16 +634,10 @@
     <t>Який вираз має закон Ома?</t>
   </si>
   <si>
-    <t>щоб запобігти розриванню зрощень</t>
-  </si>
-  <si>
     <t>Запобіжна петля на ділянці зрощення саперного проводу використовується для</t>
   </si>
   <si>
     <t>збільшення опору мережі</t>
-  </si>
-  <si>
-    <t>запобіганню розривання зрощень</t>
   </si>
   <si>
     <t>зменшення опору мережі</t>
@@ -775,6 +769,9 @@
   <si>
     <t>Для прицілювання міни МОН-50, якщо дозволяє час, використовується віха, що виготовляється у військах,
 яка встановлюється на напрямку руху, центру очікуваної групової цілі. Висота віхи від поверхні землі до поперечної планки при відстані ___ м – ___ м, при відстані ___ м – ___ м</t>
+  </si>
+  <si>
+    <t>запобігання розривання зрощень</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1066,8 @@
   </sheetPr>
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="G32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1215,7 +1212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1351,7 +1348,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
@@ -1871,7 +1868,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>141</v>
@@ -1880,7 +1877,7 @@
         <v>106</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>106</v>
@@ -2298,10 +2295,10 @@
         <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>141</v>
@@ -2733,22 +2730,22 @@
         <v>188</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="E39" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="O39" s="2" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="AA39" s="5" t="s">
         <v>69</v>
@@ -2759,19 +2756,19 @@
     </row>
     <row r="40" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>103</v>
@@ -2788,22 +2785,22 @@
     </row>
     <row r="41" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="O41" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AA41" s="5" t="s">
         <v>69</v>
@@ -2817,22 +2814,22 @@
     </row>
     <row r="42" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="O42" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AA42" s="5" t="s">
         <v>69</v>
@@ -2846,22 +2843,22 @@
     </row>
     <row r="43" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="O43" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AA43" s="5" t="s">
         <v>69</v>
@@ -2872,22 +2869,22 @@
     </row>
     <row r="44" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="O44" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AA44" s="5" t="s">
         <v>69</v>
@@ -2898,61 +2895,61 @@
     </row>
     <row r="45" spans="1:29" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O45" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="O45" s="2" t="s">
+      <c r="P45" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="Q45" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="R45" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="R45" s="2" t="s">
+      <c r="S45" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="S45" s="2" t="s">
+      <c r="T45" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="T45" s="2" t="s">
+      <c r="U45" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="V45" s="2" t="s">
+      <c r="W45" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="W45" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="AA45" s="5" t="s">
         <v>124</v>
@@ -2963,43 +2960,43 @@
     </row>
     <row r="46" spans="1:29" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="G46" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="O46" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q46" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="R46" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="T46" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S46" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="T46" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="AA46" s="5" t="s">
         <v>122</v>
@@ -3010,7 +3007,7 @@
     </row>
     <row r="47" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O47" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Added toggle button for viewing answers in admin results
</commit_message>
<xml_diff>
--- a/questions3.xlsx
+++ b/questions3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772B471-D0BA-4DD4-A429-E760172FA9A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64144317-7698-4EA5-B621-920C5DCD893C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,8 +1066,8 @@
   </sheetPr>
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed image import for questions from xlsx file
</commit_message>
<xml_diff>
--- a/questions3.xlsx
+++ b/questions3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64144317-7698-4EA5-B621-920C5DCD893C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E42B39-C9C0-4D70-91D7-1E55E1F4540C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="238">
   <si>
     <t>Question</t>
   </si>
@@ -133,21 +133,6 @@
     <t>До ініціюючих вибухових речовин відносяться:</t>
   </si>
   <si>
-    <r>
-      <t>До бризантних вибухових речовин підвищеної потужності відносяться:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>гексоген</t>
   </si>
   <si>
@@ -266,21 +251,6 @@
   </si>
   <si>
     <t>фізичний</t>
-  </si>
-  <si>
-    <r>
-      <t>Вогневий спосіб</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> застосовується для</t>
-    </r>
   </si>
   <si>
     <t>здійснення одночасного вибуху декількох зарядів, а також для бескапсюльного підриву зарядів вибухових речовин</t>
@@ -415,14 +385,6 @@
     <t>виймають із коробки КД і перевіряють його придатність шляхом огляду</t>
   </si>
   <si>
-    <t>закріплюють КД на ВШ спеціальним обтискачем, для чого беруть шнур у
-ліву руку і, притримуючи КД вказівним пальцем, накладають правою рукою обтискач так, щоб його нижня поверхня була на рівні зрізу гільзи; поступово посилюючи натискання на обтискач і повертаючи його, створюють біля краю гільзи кільцеву шийку, таким чином досягається міцність з’єднання КД зі шнуром</t>
-  </si>
-  <si>
-    <t>обрізаний під прямим кутом кінець ВШ обережно вводять у гільзу КД до
-упору в чашечку. Шнур повинен входити в гільзу легко, без натискання і обертання, які можуть призвести до підривання КД. Якщо шнур входить у гільзу досить вільно, його кінець обгортають одним шаром ізоляційної стрічки чи паперу</t>
-  </si>
-  <si>
     <t>ordering</t>
   </si>
   <si>
@@ -473,10 +435,6 @@
   <si>
     <t>трохи підняти і поворотом на 90º переставити чеку з глибокого прорізу в
 мілкий</t>
-  </si>
-  <si>
-    <t>тримаючи запалювач лівою рукою за корпус, правою рукою висмикнути
-чеку за кільце (шток запалювача направити при цьому від себе)</t>
   </si>
   <si>
     <t>Детонуючий шнур складається з</t>
@@ -558,10 +516,6 @@
     <t>від 0,9 до 1,5 Ом</t>
   </si>
   <si>
-    <t>розрахунковий опір у нагрітому стані (під час підривання) разом з
-відвідними проводами довжиною 1 м</t>
-  </si>
-  <si>
     <t>2,5 Ом</t>
   </si>
   <si>
@@ -772,6 +726,30 @@
   </si>
   <si>
     <t>запобігання розривання зрощень</t>
+  </si>
+  <si>
+    <t>відкинути ніжки вниз, розвести їх в сторони і втиснути в грунт на глибину, що забезпечує міністійке положення</t>
+  </si>
+  <si>
+    <t>порохової серцевини з однією направляючою ниткою всередині внутрішніх і зовнішніх обплетень і оболонки</t>
+  </si>
+  <si>
+    <t>обрізаний під прямим кутом кінець ВШ обережно вводять у гільзу КД до упору в чашечку. Шнур повинен входити в гільзу легко, без натискання і обертання, які можуть призвести до підривання КД. Якщо шнур входить у гільзу досить вільно, його кінець обгортають одним шаром ізоляційної стрічки чи паперу</t>
+  </si>
+  <si>
+    <t>закріплюють КД на ВШ спеціальним обтискачем, для чого беруть шнур у ліву руку і, притримуючи КД вказівним пальцем, накладають правою рукою обтискач так, щоб його нижня поверхня була на рівні зрізу гільзи; поступово посилюючи натискання на обтискач і повертаючи його, створюють біля краю гільзи кільцеву шийку, таким чином досягається міцність з’єднання КД зі шнуром</t>
+  </si>
+  <si>
+    <t>тримаючи запалювач лівою рукою за корпус, правою рукою висмикнути чеку за кільце (шток запалювача направити при цьому від себе)</t>
+  </si>
+  <si>
+    <t>розрахунковий опір у нагрітому стані (під час підривання) разом з відвідними проводами довжиною 1 м</t>
+  </si>
+  <si>
+    <t>Вогневий спосіб застосовується для …</t>
+  </si>
+  <si>
+    <t>До бризантних вибухових речовин підвищеної потужності відносяться:</t>
   </si>
 </sst>
 </file>
@@ -828,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -844,6 +822,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1067,7 +1048,7 @@
   <dimension ref="A1:AC47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1172,7 +1153,7 @@
         <v>8</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="131.25" x14ac:dyDescent="0.3">
@@ -1186,13 +1167,13 @@
         <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -1206,7 +1187,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB2" s="2">
         <v>2</v>
@@ -1217,37 +1198,37 @@
         <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>35</v>
@@ -1277,57 +1258,57 @@
         <v>2</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="L4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>35</v>
       </c>
       <c r="O4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -1345,57 +1326,57 @@
         <v>2</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -1413,27 +1394,27 @@
         <v>2</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="75" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1447,7 +1428,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB6" s="2">
         <v>2</v>
@@ -1455,37 +1436,37 @@
     </row>
     <row r="7" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="O7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1504,22 +1485,22 @@
     </row>
     <row r="8" spans="1:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="O8" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1533,33 +1514,33 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB8" s="2">
         <v>2</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="O9" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1573,33 +1554,33 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB9" s="2">
         <v>2</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="131.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="O10" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1613,48 +1594,48 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB10" s="2">
         <v>2</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="H11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1673,19 +1654,19 @@
     </row>
     <row r="12" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1696,7 +1677,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1710,7 +1691,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB12" s="2">
         <v>2</v>
@@ -1718,28 +1699,28 @@
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1747,16 +1728,16 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1774,21 +1755,21 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="168.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>78</v>
+      <c r="B14" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -1802,7 +1783,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB14" s="2">
         <v>2</v>
@@ -1810,43 +1791,43 @@
     </row>
     <row r="15" spans="1:29" ht="75" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="I15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R15" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1865,22 +1846,22 @@
     </row>
     <row r="16" spans="1:29" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>106</v>
+        <v>231</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -1894,7 +1875,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB16" s="2">
         <v>2</v>
@@ -1902,28 +1883,28 @@
     </row>
     <row r="17" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="G17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="O17" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -1937,7 +1918,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB17" s="2">
         <v>2</v>
@@ -1945,22 +1926,22 @@
     </row>
     <row r="18" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="O18" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -1974,7 +1955,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB18" s="2">
         <v>2</v>
@@ -1982,18 +1963,18 @@
     </row>
     <row r="19" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="O19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2007,7 +1988,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB19" s="2">
         <v>2</v>
@@ -2015,7 +1996,7 @@
     </row>
     <row r="20" spans="1:29" ht="206.25" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O20" s="3">
         <v>10</v>
@@ -2040,7 +2021,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB20" s="5">
         <v>2</v>
@@ -2048,31 +2029,31 @@
     </row>
     <row r="21" spans="1:29" ht="318.75" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="O21" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>121</v>
+        <v>232</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>120</v>
+        <v>233</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2083,7 +2064,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AB21" s="5">
         <v>2</v>
@@ -2091,22 +2072,22 @@
     </row>
     <row r="22" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="O22" s="3">
         <v>50</v>
@@ -2121,7 +2102,7 @@
         <v>50</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
@@ -2131,33 +2112,33 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB22" s="5">
         <v>2</v>
       </c>
       <c r="AC22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="O23" s="3">
         <v>150</v>
@@ -2172,7 +2153,7 @@
         <v>75</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
@@ -2182,33 +2163,33 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB23" s="5">
         <v>2</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="O24" s="3">
         <v>360</v>
@@ -2223,7 +2204,7 @@
         <v>65</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
@@ -2233,48 +2214,48 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB24" s="5">
         <v>2</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="150" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="O25" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
@@ -2284,7 +2265,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
       <c r="AA25" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AB25" s="5">
         <v>2</v>
@@ -2292,26 +2273,26 @@
     </row>
     <row r="26" spans="1:29" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="O26" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2321,7 +2302,7 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="AA26" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB26" s="2">
         <v>2</v>
@@ -2329,7 +2310,7 @@
     </row>
     <row r="27" spans="1:29" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2355,7 +2336,7 @@
         <v>24</v>
       </c>
       <c r="AA27" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB27" s="5">
         <v>2</v>
@@ -2363,25 +2344,25 @@
     </row>
     <row r="28" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AA28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB28" s="2">
         <v>2</v>
@@ -2389,118 +2370,118 @@
     </row>
     <row r="29" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AA29" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB29" s="2">
         <v>2</v>
       </c>
       <c r="AC29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="AA30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB30" s="2">
         <v>2</v>
       </c>
       <c r="AC30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="AA31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB31" s="2">
         <v>2</v>
       </c>
       <c r="AC31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="173.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB32" s="2">
         <v>2</v>
@@ -2508,46 +2489,46 @@
     </row>
     <row r="33" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O33" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="P33" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="AA33" s="4" t="s">
         <v>9</v>
@@ -2558,46 +2539,46 @@
     </row>
     <row r="34" spans="1:29" ht="155.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="O34" s="2" t="s">
+      <c r="R34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="S34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="T34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="R34" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="AA34" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB34" s="5">
         <v>2</v>
@@ -2605,121 +2586,121 @@
     </row>
     <row r="35" spans="1:29" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AA35" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB35" s="2">
         <v>2</v>
       </c>
       <c r="AC35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AA36" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB36" s="2">
         <v>2</v>
       </c>
       <c r="AC36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AA37" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB37" s="2">
         <v>2</v>
       </c>
       <c r="AC37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AA38" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB38" s="2">
         <v>2</v>
@@ -2727,28 +2708,28 @@
     </row>
     <row r="39" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AA39" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB39" s="2">
         <v>2</v>
@@ -2756,112 +2737,112 @@
     </row>
     <row r="40" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AA40" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB40" s="2">
         <v>2</v>
       </c>
       <c r="AC40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AA41" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB41" s="2">
         <v>2</v>
       </c>
       <c r="AC41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AA42" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB42" s="2">
         <v>2</v>
       </c>
       <c r="AC42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="AA43" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB43" s="2">
         <v>2</v>
@@ -2869,25 +2850,25 @@
     </row>
     <row r="44" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AA44" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="2">
         <v>2</v>
@@ -2895,64 +2876,64 @@
     </row>
     <row r="45" spans="1:29" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q45" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="O45" s="2" t="s">
+      <c r="R45" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="S45" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="T45" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="R45" s="2" t="s">
+      <c r="U45" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="S45" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="T45" s="2" t="s">
+      <c r="W45" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="U45" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="W45" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="AA45" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB45" s="5">
         <v>2</v>
@@ -2960,46 +2941,46 @@
     </row>
     <row r="46" spans="1:29" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>230</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AA46" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AB46" s="5">
         <v>2</v>
@@ -3007,7 +2988,7 @@
     </row>
     <row r="47" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="O47" s="2">
         <v>10</v>
@@ -3022,7 +3003,7 @@
         <v>1.6</v>
       </c>
       <c r="AA47" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB47" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
Added questions4 and questions5
</commit_message>
<xml_diff>
--- a/questions3.xlsx
+++ b/questions3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258B37B9-4277-47CE-B110-F4C1E5B71EDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90041969-EA30-4D8A-9B51-B75DE315CBF0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="318">
   <si>
     <t>Question</t>
   </si>
@@ -277,13 +277,6 @@
 використовуються для підривання різних фігурних елементів конструкцій"</t>
   </si>
   <si>
-    <t>До яких зарядів відноситься це визначення? 
-"Заряди, які мають форму витягнутих паралелепіпедів
-чи циліндрів, довжина яких більше ніж у п’ять разів перевищує їх найменші
-поперечні розміри, при цьому висота зарядів, що мають форму
-паралелепіпедів, не повинна перевищувати їх ширину"</t>
-  </si>
-  <si>
     <t>За формою заряди бувають</t>
   </si>
   <si>
@@ -314,9 +307,6 @@
     <t>електродетонатори</t>
   </si>
   <si>
-    <t>Яка довжина бухти вогнепровідного шнура</t>
-  </si>
-  <si>
     <t>5 метрів</t>
   </si>
   <si>
@@ -333,9 +323,6 @@
   </si>
   <si>
     <t>10 метрів</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Вогнепровідний шнур складається з</t>
   </si>
   <si>
     <t>порохової серцевини з
@@ -343,9 +330,6 @@
 оболонки</t>
   </si>
   <si>
-    <t>Швидкість горіння вогнепровідного шнура на відкритому повітрі становить приблизно</t>
-  </si>
-  <si>
     <t>1 см/с</t>
   </si>
   <si>
@@ -440,17 +424,7 @@
     <t>серцевини бризантної ВР (тену) з двома направляючими нитками і ряду внутрішніх і зовнішніх обплетень, покритих вологоізолюючою оболонкою</t>
   </si>
   <si>
-    <t>Діаметр ДШ дорівнює ___–___ мм. ДШ підривається зі швидкістю не менше ___ метрів за секунду. Його
-слід оберігати від механічних пошкоджень, а також від дії вологи і вогню; від вогню ДШ може загоратися і повільно горіти; у разі прострілювання кулею він
-може детонувати. ДШ відрізками довжиною ___ м зберігається згорнутим у бухти з покритими мастикою кінцями в сухих прохолодних приміщеннях окремо від ВШ і зарядів. Під водою ДШ марки ДШ-В можна підривати за умови перебування його
-там не більше ___ годин</t>
-  </si>
-  <si>
     <t>4-5 витків</t>
-  </si>
-  <si>
-    <t>Скількома витками детонуючого шнура необхідно обмотати шашку пресованого
-тротилу щоб можна було підірвати її без КД?</t>
   </si>
   <si>
     <t>2-3 витка</t>
@@ -750,6 +724,266 @@
   <si>
     <t>Для прицілювання міни МОН-50, якщо дозволяє час, використовується віха, що виготовляється у військах,
 яка встановлюється на напрямку руху, центру очікуваної групової цілі. Висота віхи від поверхні землі до поперечної планки при відстані ___ м дорівнює ___ м, при відстані ___ м – ___ м</t>
+  </si>
+  <si>
+    <t xml:space="preserve">При проведенні підривних робіт з ЕДП уповільненої дії до зарядів, що відмовили, дозволяється підходити не раніше ніж через </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Необхідно розміщувати проводи ЕВМ від електричних станцій, підстанцій, високовольтних ліній, електрифікованих залізниць і потужних радіостанцій не ближче ніж  </t>
+  </si>
+  <si>
+    <t>200 метрів</t>
+  </si>
+  <si>
+    <t>300 метрів</t>
+  </si>
+  <si>
+    <t>протипіхотна</t>
+  </si>
+  <si>
+    <t>протитанкова</t>
+  </si>
+  <si>
+    <t>осколкова</t>
+  </si>
+  <si>
+    <t>фугасна</t>
+  </si>
+  <si>
+    <t>кумулятивна</t>
+  </si>
+  <si>
+    <t>направленої дії</t>
+  </si>
+  <si>
+    <t>кругової дії</t>
+  </si>
+  <si>
+    <t>об'єктна</t>
+  </si>
+  <si>
+    <t>Яка довжина бухти вогнепровідного шнура ОШП</t>
+  </si>
+  <si>
+    <t>Яка довжина бухти вогнепровідного шнура М-700 (США)?</t>
+  </si>
+  <si>
+    <t>5,1 метрів</t>
+  </si>
+  <si>
+    <t>10,1 метрів</t>
+  </si>
+  <si>
+    <t>15,2 метрів</t>
+  </si>
+  <si>
+    <t>20,3 метрів</t>
+  </si>
+  <si>
+    <t>25,5 метрів</t>
+  </si>
+  <si>
+    <t>До яких зарядів відноситься це визначення? 
+"Заряди, які мають форму витягнутих паралелепіпедів
+чи циліндрів, довжина яких більше ніж у п’ять разів перевищує їх найменші поперечні розміри, при цьому висота зарядів, що мають форму паралелепіпедів, не повинна перевищувати їх ширину"</t>
+  </si>
+  <si>
+    <t>Скількома витками детонуючого шнура необхідно обмотати шашку пресованого тротилу щоб можна було підірвати її без КД?</t>
+  </si>
+  <si>
+    <t>Мінімальний відрізок ОШП під час практичних підривних роботах (для навчання) повинен бути не менше</t>
+  </si>
+  <si>
+    <t>10 см</t>
+  </si>
+  <si>
+    <t>15 см</t>
+  </si>
+  <si>
+    <t>20 см</t>
+  </si>
+  <si>
+    <t>25 см</t>
+  </si>
+  <si>
+    <t>40 см</t>
+  </si>
+  <si>
+    <t>50 см</t>
+  </si>
+  <si>
+    <t>Мінімальний відрізок ОШП під час підриву льоду повинен бути не менше</t>
+  </si>
+  <si>
+    <t>Мінімальний відрізок ОШП в бойовій обстановці повинен бути не менше</t>
+  </si>
+  <si>
+    <t>Швидкість горіння вогнепровідного шнура ОШП на відкритому повітрі становить приблизно</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Вогнепровідний шнур ОШП складається з</t>
+  </si>
+  <si>
+    <t>Швидкість горіння вогнепровідного шнура М-700 (США) на відкритому повітрі становить приблизно</t>
+  </si>
+  <si>
+    <t>1,5 см/с</t>
+  </si>
+  <si>
+    <t>2 см/с</t>
+  </si>
+  <si>
+    <t>здійснення одночасного підриву декількох зарядів, а також для безкапсульного підривання зарядів ВР, закладених в важкодоступних місцях</t>
+  </si>
+  <si>
+    <t>для здійснення одночасного підриву декількох зарядів, а також для безкапсульного підривання зарядів ВР, закладених в важкодоступних місцях</t>
+  </si>
+  <si>
+    <t>Діаметр ДШ-В дорівнює ___–___ мм. ДШ-В підривається зі швидкістю не менше ___ метрів за секунду. Його слід оберігати від механічних пошкоджень, а також від дії вологи і вогню; від вогню ДШ може загоратися і повільно горіти; у разі прострілювання кулею він може детонувати. ДШ відрізками довжиною ___ м зберігається згорнутим у бухти з покритими мастикою кінцями в сухих прохолодних приміщеннях окремо від ВШ і зарядів. В одному погонному метрі  ДШ-В міститься ___ г вибухової речовини ТЕН. Під водою ДШ марки ДШ-В можна підривати за умови перебування його там не більше ___ годин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Діаметр ДШЕ-6 дорівнює ___ мм. ДШЕ-6 підривається зі швидкістю не менше ___ метрів за секунду. ДШЕ-6 відрізками довжиною ___ м зберігається згорнутим у бухти з покритими мастикою кінцями в сухих прохолодних приміщеннях окремо від ВШ і зарядів. В одному погонному метрі  ДШЕ-6 міститься ___ г вибухової речовини </t>
+  </si>
+  <si>
+    <t>Якими способами здійснюються зростки ДШ?</t>
+  </si>
+  <si>
+    <t>Вариант 1</t>
+  </si>
+  <si>
+    <t>Вариант 2</t>
+  </si>
+  <si>
+    <t>Вариант 3</t>
+  </si>
+  <si>
+    <t>Вариант 4</t>
+  </si>
+  <si>
+    <t>Вариант 5</t>
+  </si>
+  <si>
+    <t>Вариант 6</t>
+  </si>
+  <si>
+    <t>Який вариант зростки ДШ внакладку правильний?</t>
+  </si>
+  <si>
+    <t>Вариант А</t>
+  </si>
+  <si>
+    <t>Вариант Б</t>
+  </si>
+  <si>
+    <t>Підходити до зарядів, що відмовили при електричному способі підриву  дозволяється не раніше ніж через</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Якщо заряди, з’єднані ДШ відмовили, то підходити до них дозволяється тільки одній особі і не раніше ніж через </t>
+  </si>
+  <si>
+    <t>Електроспалахувачі  призначені  для</t>
+  </si>
+  <si>
+    <t>ініціювання  капсулів-детонаторів  і спалахування  порохових  зарядів</t>
+  </si>
+  <si>
+    <t>ініціювання вибуху підривних зарядів</t>
+  </si>
+  <si>
+    <t>Електродетонатори  призначені  для</t>
+  </si>
+  <si>
+    <t>передачі електричного імпульсу від джерела живлення до ЕД</t>
+  </si>
+  <si>
+    <t>Який буде опір саперного дроту СПП-2 якщо його довжина складає 100 метрів?</t>
+  </si>
+  <si>
+    <t>Який буде опір саперного дроту СПП-2 якщо його довжина складає 200 метрів?</t>
+  </si>
+  <si>
+    <t>15 Ом</t>
+  </si>
+  <si>
+    <t>7,5 Ом</t>
+  </si>
+  <si>
+    <t>Який буде опір саперного дроту СПП-2 якщо його довжина складає 2 км?</t>
+  </si>
+  <si>
+    <t>75 Ом</t>
+  </si>
+  <si>
+    <t>150 Ом</t>
+  </si>
+  <si>
+    <t>Підривні машинки призначені для</t>
+  </si>
+  <si>
+    <t>ініціювання електродетонаторів нормальної чутливості (ЕДП та їх аналогів) при проведенні підривних робіт</t>
+  </si>
+  <si>
+    <t>передачі електричного імпульсу від джерела живлення до вибухового заряду</t>
+  </si>
+  <si>
+    <t>Тактико-технічні характеристики підривної машинки  «ВИХОР»</t>
+  </si>
+  <si>
+    <t>Максимальна кількість ЕД при послідовному з’єднанні</t>
+  </si>
+  <si>
+    <t>Максимальна кількість ЕД при паралельному з’єднанні</t>
+  </si>
+  <si>
+    <t>Максимальний опір електровибухової мережі, Ом</t>
+  </si>
+  <si>
+    <t>Напруга розряду, В</t>
+  </si>
+  <si>
+    <t>Вага, г</t>
+  </si>
+  <si>
+    <t>ініціювання електродетонаторів при проведенні підривних робіт</t>
+  </si>
+  <si>
+    <t>Тактико-технічні характеристики підривної машинки КПМ-3</t>
+  </si>
+  <si>
+    <t>Максимальний опір електровибухової мережі при послідовному з’єднанні, Ом</t>
+  </si>
+  <si>
+    <t>Максимальний опір електровибухової мережі при паралельному з’єднанні, Ом</t>
+  </si>
+  <si>
+    <t>Напруга, В</t>
+  </si>
+  <si>
+    <t>Тактико-технічні характеристики підривної машинки ПМ-4</t>
+  </si>
+  <si>
+    <t>Довжина проводової лінії, м</t>
+  </si>
+  <si>
+    <t>вистрибуюча</t>
+  </si>
+  <si>
+    <t>протигусенична</t>
+  </si>
+  <si>
+    <t>протибортова</t>
+  </si>
+  <si>
+    <t>протипранспортна</t>
+  </si>
+  <si>
+    <t>Picture38</t>
+  </si>
+  <si>
+    <t>Picture39</t>
+  </si>
+  <si>
+    <t>Дайте повну характеристику міни МОН-50</t>
   </si>
 </sst>
 </file>
@@ -809,23 +1043,25 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,13 +1281,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC47"/>
+  <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA66" sqref="AA66:AB66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="2"/>
     <col min="2" max="2" width="65.42578125" style="2" customWidth="1"/>
@@ -1067,7 +1303,7 @@
     <col min="28" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1156,7 +1392,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="131.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="131.25" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1186,14 +1422,14 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
@@ -1261,9 +1497,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>41</v>
@@ -1329,7 +1565,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
@@ -1397,7 +1633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="75" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>47</v>
       </c>
@@ -1427,19 +1663,19 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="5" t="s">
+      <c r="AA6" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>80</v>
@@ -1454,7 +1690,7 @@
         <v>82</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>80</v>
@@ -1483,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>78</v>
       </c>
@@ -1513,7 +1749,7 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="5" t="s">
+      <c r="AA8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB8" s="2">
@@ -1523,7 +1759,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
@@ -1553,7 +1789,7 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="5" t="s">
+      <c r="AA9" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB9" s="2">
@@ -1563,9 +1799,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="131.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>251</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>80</v>
@@ -1593,7 +1829,7 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="5" t="s">
+      <c r="AA10" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB10" s="2">
@@ -1603,7 +1839,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
@@ -1620,7 +1856,7 @@
         <v>53</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>56</v>
@@ -1652,7 +1888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>62</v>
       </c>
@@ -1690,14 +1926,14 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="5" t="s">
+      <c r="AA12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>68</v>
       </c>
@@ -1754,22 +1990,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="168.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
-        <v>227</v>
+    <row r="14" spans="1:29" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="O14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -1782,52 +2020,52 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="5" t="s">
+      <c r="AA14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="I15" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="O15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1844,24 +2082,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>102</v>
+        <v>263</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -1874,37 +2112,37 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="5" t="s">
+      <c r="AA16" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:29" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="G17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="O17" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -1917,31 +2155,31 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="5" t="s">
+      <c r="AA17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="O18" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -1954,27 +2192,27 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="5" t="s">
+      <c r="AA18" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:29" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="O19" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -1987,16 +2225,16 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="5" t="s">
+      <c r="AA19" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="206.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:29" ht="193.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O20" s="3">
         <v>10</v>
@@ -2020,40 +2258,40 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB20" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" ht="318.75" x14ac:dyDescent="0.3">
+      <c r="AA20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" ht="270.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2063,47 +2301,42 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB21" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="AA21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>118</v>
+        <v>253</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>120</v>
+        <v>254</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>123</v>
+        <v>255</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="O22" s="3">
-        <v>50</v>
-      </c>
-      <c r="P22" s="3">
-        <v>40</v>
-      </c>
-      <c r="Q22">
-        <v>55</v>
-      </c>
-      <c r="R22">
-        <v>50</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -2111,50 +2344,45 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
-      <c r="AA22" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB22" s="5">
+      <c r="AA22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB22" s="2">
         <v>2</v>
       </c>
       <c r="AC22" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:29" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>126</v>
+        <v>260</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>254</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>123</v>
+        <v>255</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="O23" s="3">
-        <v>150</v>
-      </c>
-      <c r="P23" s="3">
-        <v>100</v>
-      </c>
-      <c r="Q23">
-        <v>150</v>
-      </c>
-      <c r="R23">
-        <v>75</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2162,50 +2390,45 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
-      <c r="AA23" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB23" s="5">
+      <c r="AA23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB23" s="2">
         <v>2</v>
       </c>
       <c r="AC23" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:29" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>127</v>
+        <v>261</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>120</v>
+        <v>254</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>123</v>
+        <v>255</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="O24" s="3">
-        <v>360</v>
-      </c>
-      <c r="P24" s="3">
-        <v>300</v>
-      </c>
-      <c r="Q24">
-        <v>100</v>
-      </c>
-      <c r="R24">
-        <v>65</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2213,50 +2436,45 @@
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
-      <c r="AA24" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB24" s="5">
+      <c r="AA24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB24" s="2">
         <v>2</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="150" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:29" ht="37.5" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>131</v>
+        <v>247</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>130</v>
+        <v>248</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>133</v>
+        <v>249</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>225</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -2264,35 +2482,31 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
-      <c r="AA25" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB25" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
-        <v>134</v>
+      <c r="AA25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" ht="37.5" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>192</v>
+        <v>101</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+        <v>266</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="O26" s="3" t="s">
-        <v>135</v>
+        <v>265</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2301,312 +2515,372 @@
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="AA26" s="5" t="s">
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O27" s="3">
+        <v>50</v>
+      </c>
+      <c r="P27" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>55</v>
+      </c>
+      <c r="R27" s="6">
+        <v>50</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O28" s="3">
+        <v>150</v>
+      </c>
+      <c r="P28" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>150</v>
+      </c>
+      <c r="R28" s="6">
+        <v>75</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O29" s="3">
+        <v>360</v>
+      </c>
+      <c r="P29" s="3">
+        <v>300</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>100</v>
+      </c>
+      <c r="R29" s="6">
+        <v>65</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="O31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="AA31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" ht="258" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="O32" s="2">
+        <v>5</v>
+      </c>
+      <c r="P32" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>6500</v>
+      </c>
+      <c r="R32" s="2">
+        <v>50</v>
+      </c>
+      <c r="S32" s="2">
+        <v>13</v>
+      </c>
+      <c r="T32" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="O33" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="P33" s="2">
+        <v>6200</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>50</v>
+      </c>
+      <c r="R33" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="O27" s="2">
-        <v>5</v>
-      </c>
-      <c r="P27" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>6500</v>
-      </c>
-      <c r="R27" s="2">
-        <v>50</v>
-      </c>
-      <c r="S27" s="2">
-        <v>24</v>
-      </c>
-      <c r="AA27" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB27" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB28" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA29" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB29" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA30" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB30" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC30" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB31" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC31" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" ht="173.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB32" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="S33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB33" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" ht="155.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AA34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB34" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="O35" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA35" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA35" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB35" s="2">
@@ -2616,29 +2890,29 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA36" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB36" s="2">
@@ -2648,29 +2922,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AA37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA37" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB37" s="2">
@@ -2680,332 +2954,1093 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="B38" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="O42" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="AA42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="O43" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="AA43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC46" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC47" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB49" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC49" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB50" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC50" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB51" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC51" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB52" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="O54" s="2">
+        <v>50</v>
+      </c>
+      <c r="P54" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>150</v>
+      </c>
+      <c r="R54" s="2">
+        <v>400</v>
+      </c>
+      <c r="S54" s="2">
+        <v>650</v>
+      </c>
+      <c r="AA54" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB54" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC54" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="O55" s="2">
+        <v>200</v>
+      </c>
+      <c r="P55" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>600</v>
+      </c>
+      <c r="R55" s="2">
+        <v>15</v>
+      </c>
+      <c r="S55" s="2">
+        <v>1600</v>
+      </c>
+      <c r="T55" s="2">
+        <v>2300</v>
+      </c>
+      <c r="AA55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB55" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC55" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="O56" s="2">
+        <v>5</v>
+      </c>
+      <c r="P56" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>20</v>
+      </c>
+      <c r="R56" s="2">
+        <v>6</v>
+      </c>
+      <c r="S56" s="2">
+        <v>50</v>
+      </c>
+      <c r="T56" s="2">
+        <v>410</v>
+      </c>
+      <c r="AA56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC56" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AA38" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB38" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA57" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB57" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC57" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB58" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC58" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB59" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC59" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA60" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA61" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB61" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB62" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA63" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB63" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA64" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB64" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:28" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AA65" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB65" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="AA39" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB39" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA40" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB40" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC40" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB41" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC41" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB42" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC42" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB43" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
+      <c r="D66" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O66" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="P66" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q66" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB66" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="E67" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O67" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O44" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="AA44" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB44" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
+      <c r="P67" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q67" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I45" s="2" t="s">
+      <c r="R67" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="T67" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="U67" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="V67" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="W67" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA67" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB67" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="C68" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="E68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="O45" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="S45" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="U45" s="2" t="s">
+      <c r="O68" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="V45" s="2" t="s">
+      <c r="P68" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q68" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="W45" s="2" t="s">
+      <c r="R68" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="S68" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AA45" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB45" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="2" t="s">
+      <c r="T68" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="S46" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="T46" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="AA46" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB46" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="O47" s="2">
+      <c r="AA68" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="O69" s="2">
         <v>10</v>
       </c>
-      <c r="P47" s="2">
+      <c r="P69" s="2">
         <v>0.6</v>
       </c>
-      <c r="Q47" s="2">
+      <c r="Q69" s="2">
         <v>30</v>
       </c>
-      <c r="R47" s="2">
+      <c r="R69" s="2">
         <v>1.6</v>
       </c>
-      <c r="AA47" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB47" s="5">
+      <c r="AA69" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB69" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>